<commit_message>
Updating. I think it almost works now!
</commit_message>
<xml_diff>
--- a/parameters/mcd_grid_variables.xlsx
+++ b/parameters/mcd_grid_variables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaronberliner/MCD/mcd-python/redSun/parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9968B482-818B-4849-A9B7-7AA26843526B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20BADFB3-117B-6846-9C1F-E165DD592C46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-46920" yWindow="4100" windowWidth="19200" windowHeight="21140" xr2:uid="{80499892-240A-CD48-8631-CADB428A502E}"/>
+    <workbookView xWindow="-46920" yWindow="4100" windowWidth="19200" windowHeight="21140" activeTab="1" xr2:uid="{80499892-240A-CD48-8631-CADB428A502E}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="122">
   <si>
     <t>name</t>
   </si>
@@ -393,6 +393,12 @@
   </si>
   <si>
     <t>pp_NO2</t>
+  </si>
+  <si>
+    <t>degrees north</t>
+  </si>
+  <si>
+    <t>degrees east</t>
   </si>
 </sst>
 </file>
@@ -755,7 +761,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31F9C618-BF1D-5B4A-A55D-FB1B6A086F61}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -1147,10 +1153,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A91FAC5B-FE6C-E442-BEF6-68AC2DC844CE}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1178,7 +1184,7 @@
         <v>70</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1189,7 +1195,7 @@
         <v>71</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1234,17 +1240,6 @@
       </c>
       <c r="C7" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>66</v>
-      </c>
-      <c r="B8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C8" t="s">
-        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding datastructure builder notebook. Trying to get back on the horse.
</commit_message>
<xml_diff>
--- a/parameters/mcd_grid_variables.xlsx
+++ b/parameters/mcd_grid_variables.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaronberliner/MCD/mcd-python/redSun/parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20BADFB3-117B-6846-9C1F-E165DD592C46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D9B15BA-7959-9F48-AF10-1E1BA1B5F4E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-46920" yWindow="4100" windowWidth="19200" windowHeight="21140" activeTab="1" xr2:uid="{80499892-240A-CD48-8631-CADB428A502E}"/>
+    <workbookView xWindow="-46920" yWindow="4100" windowWidth="19200" windowHeight="21140" xr2:uid="{80499892-240A-CD48-8631-CADB428A502E}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
     <sheet name="coords" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -761,8 +764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31F9C618-BF1D-5B4A-A55D-FB1B6A086F61}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1155,7 +1158,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A91FAC5B-FE6C-E442-BEF6-68AC2DC844CE}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>

</xml_diff>